<commit_message>
subject change & change back
</commit_message>
<xml_diff>
--- a/records_maps/Capstone Maps/salliebingham-map2019.xlsx
+++ b/records_maps/Capstone Maps/salliebingham-map2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfreedma/Documents/GitHub/zinecat.org/records_maps/Capstone Maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BC6ABE-A712-9540-80FC-A5FD387E07CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF496C0-F75C-2F43-BCB0-DFA87CE01452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="21600" windowHeight="14280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,16 @@
     <definedName name="table">'Drop-down Lists'!$F$1:$F$16</definedName>
     <definedName name="YES_NO">'Drop-down Lists'!$D$1:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -338,7 +344,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -392,12 +398,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFE01E5A"/>
-      <name val="Monaco"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -419,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -470,7 +470,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +757,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="137" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,11 +1253,9 @@
         <v>88</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -1292,9 +1289,11 @@
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="20" t="s">
-        <v>92</v>
+      <c r="F15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>

</xml_diff>

<commit_message>
sallie bingham delimiter changed to ;
</commit_message>
<xml_diff>
--- a/records_maps/Capstone Maps/salliebingham-map2019.xlsx
+++ b/records_maps/Capstone Maps/salliebingham-map2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfreedma/Documents/GitHub/zinecat.org/records_maps/Capstone Maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39717A11-603F-3D4A-B016-E19ACDC707F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237F9EF9-C6E3-804A-959B-7DA8F2333404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="460" windowWidth="24380" windowHeight="15160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="table">'Drop-down Lists'!$F$1:$F$16</definedName>
     <definedName name="YES_NO">'Drop-down Lists'!$D$1:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -316,9 +316,6 @@
     <t>listItemSplitter</t>
   </si>
   <si>
-    <t>{"delimiter": ",", "relationshipType": "is described by", "list": "zinecatsubject"}</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>salliebingham-map2019</t>
+  </si>
+  <si>
+    <t>{"delimiter": ";", "relationshipType": "is described by", "list": "zinecatsubject"}</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="137" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,10 +979,10 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -1017,10 +1017,10 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1086,10 +1086,10 @@
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1182,7 +1182,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1255,7 +1255,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -1285,7 +1285,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -1293,7 +1293,7 @@
         <v>89</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1411,13 +1411,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="12" t="s">
@@ -1518,7 +1518,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>60</v>
@@ -1556,7 +1556,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>63</v>

</xml_diff>